<commit_message>
Updated answer 2b, mentioning T-test
</commit_message>
<xml_diff>
--- a/Task1.xlsx
+++ b/Task1.xlsx
@@ -230,9 +230,98 @@
 Independent variable causes the change in dependent variable and vice-a-versa is not true. "</t>
   </si>
   <si>
+    <t>d-bar: -7.964791667</t>
+  </si>
+  <si>
+    <t>x-bar (Confruent)</t>
+  </si>
+  <si>
+    <t>x-bar (InConfruent)</t>
+  </si>
+  <si>
+    <t>degree of freedom</t>
+  </si>
+  <si>
+    <t>Sample Size</t>
+  </si>
+  <si>
+    <t>point estimate</t>
+  </si>
+  <si>
+    <t>S (stndard deviation of defferences)</t>
+  </si>
+  <si>
+    <t>d-bar( mean of differences)</t>
+  </si>
+  <si>
+    <t>variance of diffences</t>
+  </si>
+  <si>
+    <t>Di-Dbar</t>
+  </si>
+  <si>
+    <t>(Di-Dbar) ^2</t>
+  </si>
+  <si>
+    <t>Variance of Differences: 23.66654087</t>
+  </si>
+  <si>
+    <t>Standard Devication of Differences: 4.86482691</t>
+  </si>
+  <si>
+    <t>Standard Error of Mean Diff</t>
+  </si>
+  <si>
+    <t>Standard Error of Mean Diff: 0.993028635</t>
+  </si>
+  <si>
+    <t>t-statistics</t>
+  </si>
+  <si>
+    <t>t-statistics: -8.020706944</t>
+  </si>
+  <si>
+    <t>margin of error</t>
+  </si>
+  <si>
+    <t>Cohen's d</t>
+  </si>
+  <si>
+    <t>Confidance Interval</t>
+  </si>
+  <si>
+    <t>Left:</t>
+  </si>
+  <si>
+    <t>Right:</t>
+  </si>
+  <si>
+    <t>Cohen's d: -1.637219949</t>
+  </si>
+  <si>
+    <t>Confidance Interval: -10.01936791 to -5.910215421</t>
+  </si>
+  <si>
+    <t>Consclusion: 
+1. We Reject the Null hypothesis, that means there is significant difference in result outcome  beteen Congruent and Incongruent word condition tests results.
+2. Based on the Confidence interwal we can say that all the participants performes 5 to 10 less errors in the test given on Congruent word coditions.</t>
+  </si>
+  <si>
+    <t>Result Expectations: Yes these results match my expectations as the Incongruent word condition based test was way more difficult than the other.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The two-tailed P value is less than 0.0001 
+   By conventional criteria, this difference is considered to be extremely statistically significant. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">p-value: The two-tailed P value is less than 0.0001 
+By conventional criteria, this difference is considered to be extremely statistically significant. </t>
+  </si>
+  <si>
     <t xml:space="preserve">Since Our Null Hypothesis is MUc = MUi, that means different word conditions doesnot affect our output. So we will check the Standard deviation of the sample and check if its t-stetistical value is within the t-critical bounds (as in whichever direction the t-statistical value goes, if the variation is in t-critical region, we can say that the type of test conditions have definately affected the test results).
 Reason for taking t-test  insted of z-test is we don't know the population mean and poulation's standard devication. 
 Stetistical test which I expect to perform is:
+t-test: Since each participant completes each of the word condition tests, we will be performing dependent t-test for paired samples. As two tasks are given to same candidate and output is recorded on both the conditions. 
 Measures of Center: 
 1. Mean of both the "congruent words condition and an incongruent words condition" test ouput. This gives us the average test scores.
 2. Mod: Gives us the most frequent value in the data set
@@ -244,94 +333,6 @@
 2. Find Standard deviation: This defines how far from the average each score is.
 Also, an assumption is made that all these test were performed at same time for all the participants in similar conditions (for example similar lighing condition, same time, etc)
 </t>
-  </si>
-  <si>
-    <t>d-bar: -7.964791667</t>
-  </si>
-  <si>
-    <t>x-bar (Confruent)</t>
-  </si>
-  <si>
-    <t>x-bar (InConfruent)</t>
-  </si>
-  <si>
-    <t>degree of freedom</t>
-  </si>
-  <si>
-    <t>Sample Size</t>
-  </si>
-  <si>
-    <t>point estimate</t>
-  </si>
-  <si>
-    <t>S (stndard deviation of defferences)</t>
-  </si>
-  <si>
-    <t>d-bar( mean of differences)</t>
-  </si>
-  <si>
-    <t>variance of diffences</t>
-  </si>
-  <si>
-    <t>Di-Dbar</t>
-  </si>
-  <si>
-    <t>(Di-Dbar) ^2</t>
-  </si>
-  <si>
-    <t>Variance of Differences: 23.66654087</t>
-  </si>
-  <si>
-    <t>Standard Devication of Differences: 4.86482691</t>
-  </si>
-  <si>
-    <t>Standard Error of Mean Diff</t>
-  </si>
-  <si>
-    <t>Standard Error of Mean Diff: 0.993028635</t>
-  </si>
-  <si>
-    <t>t-statistics</t>
-  </si>
-  <si>
-    <t>t-statistics: -8.020706944</t>
-  </si>
-  <si>
-    <t>margin of error</t>
-  </si>
-  <si>
-    <t>Cohen's d</t>
-  </si>
-  <si>
-    <t>Confidance Interval</t>
-  </si>
-  <si>
-    <t>Left:</t>
-  </si>
-  <si>
-    <t>Right:</t>
-  </si>
-  <si>
-    <t>Cohen's d: -1.637219949</t>
-  </si>
-  <si>
-    <t>Confidance Interval: -10.01936791 to -5.910215421</t>
-  </si>
-  <si>
-    <t>Consclusion: 
-1. We Reject the Null hypothesis, that means there is significant difference in result outcome  beteen Congruent and Incongruent word condition tests results.
-2. Based on the Confidence interwal we can say that all the participants performes 5 to 10 less errors in the test given on Congruent word coditions.</t>
-  </si>
-  <si>
-    <t>Result Expectations: Yes these results match my expectations as the Incongruent word condition based test was way more difficult than the other.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The two-tailed P value is less than 0.0001 
-   By conventional criteria, this difference is considered to be extremely statistically significant. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">p-value: The two-tailed P value is less than 0.0001 
-By conventional criteria, this difference is considered to be extremely statistically significant. </t>
   </si>
 </sst>
 </file>
@@ -922,8 +923,8 @@
   </sheetPr>
   <dimension ref="A1:L151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="D162" sqref="D162"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -991,7 +992,7 @@
     <row r="11" spans="1:12" ht="409" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="B11" s="8" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="48" x14ac:dyDescent="0.2">
@@ -1021,7 +1022,7 @@
       <c r="K15" s="12"/>
       <c r="L15" s="6"/>
     </row>
-    <row r="16" spans="1:12" ht="80" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="13" t="s">
         <v>26</v>
@@ -2388,10 +2389,10 @@
         <v>37</v>
       </c>
       <c r="G106" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="H106" s="18" t="s">
         <v>60</v>
-      </c>
-      <c r="H106" s="18" t="s">
-        <v>61</v>
       </c>
       <c r="I106" s="14"/>
       <c r="J106" s="15"/>
@@ -2453,7 +2454,7 @@
     <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" s="7"/>
       <c r="B109" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C109" s="14"/>
       <c r="D109" s="2">
@@ -2480,7 +2481,7 @@
     <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" s="7"/>
       <c r="B110" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C110" s="14"/>
       <c r="D110" s="2">
@@ -2507,7 +2508,7 @@
     <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" s="7"/>
       <c r="B111" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C111" s="14"/>
       <c r="D111" s="2">
@@ -2534,7 +2535,7 @@
     <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" s="7"/>
       <c r="B112" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C112" s="14"/>
       <c r="D112" s="2">
@@ -2561,7 +2562,7 @@
     <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" s="7"/>
       <c r="B113" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C113" s="14"/>
       <c r="D113" s="2">
@@ -2588,7 +2589,7 @@
     <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" s="7"/>
       <c r="B114" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C114" s="14"/>
       <c r="D114" s="2">
@@ -2615,7 +2616,7 @@
     <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" s="7"/>
       <c r="B115" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C115" s="14"/>
       <c r="D115" s="2">
@@ -2642,7 +2643,7 @@
     <row r="116" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A116" s="7"/>
       <c r="B116" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C116" s="14"/>
       <c r="D116" s="2">
@@ -2696,7 +2697,7 @@
     <row r="118" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A118" s="7"/>
       <c r="B118" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C118" s="14"/>
       <c r="D118" s="2">
@@ -2723,7 +2724,7 @@
     <row r="119" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A119" s="7"/>
       <c r="B119" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C119" s="14"/>
       <c r="D119" s="2">
@@ -3026,7 +3027,7 @@
       <c r="A131" s="7"/>
       <c r="B131" s="14"/>
       <c r="C131" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D131" s="17">
         <f>AVERAGE(D107:D130)</f>
@@ -3043,7 +3044,7 @@
       <c r="A132" s="7"/>
       <c r="B132" s="14"/>
       <c r="C132" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D132" s="3"/>
       <c r="E132" s="3">
@@ -3060,7 +3061,7 @@
       <c r="A133" s="7"/>
       <c r="B133" s="14"/>
       <c r="C133" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D133" s="3">
         <v>24</v>
@@ -3076,7 +3077,7 @@
       <c r="A134" s="7"/>
       <c r="B134" s="14"/>
       <c r="C134" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D134" s="3">
         <f>D133-1</f>
@@ -3093,7 +3094,7 @@
       <c r="A135" s="7"/>
       <c r="B135" s="14"/>
       <c r="C135" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D135" s="3">
         <f>D131-E132</f>
@@ -3110,7 +3111,7 @@
       <c r="A136" s="7"/>
       <c r="B136" s="14"/>
       <c r="C136" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D136" s="3">
         <f>AVERAGE(F107:F130)</f>
@@ -3127,7 +3128,7 @@
       <c r="A137" s="7"/>
       <c r="B137" s="14"/>
       <c r="C137" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D137" s="3">
         <f>SUM(H107:H130)/D134</f>
@@ -3144,7 +3145,7 @@
       <c r="A138" s="7"/>
       <c r="B138" s="14"/>
       <c r="C138" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D138" s="3">
         <f>SQRT(D137)</f>
@@ -3161,7 +3162,7 @@
       <c r="A139" s="7"/>
       <c r="B139" s="14"/>
       <c r="C139" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D139" s="3">
         <f>D138/SQRT(D133)</f>
@@ -3178,7 +3179,7 @@
       <c r="A140" s="7"/>
       <c r="B140" s="14"/>
       <c r="C140" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D140" s="3">
         <f>D136/D139</f>
@@ -3203,7 +3204,7 @@
       <c r="A141" s="7"/>
       <c r="B141" s="14"/>
       <c r="C141" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D141" s="3">
         <f>I140*D139</f>
@@ -3220,7 +3221,7 @@
       <c r="A142" s="7"/>
       <c r="B142" s="14"/>
       <c r="C142" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D142" s="3">
         <f>D136/D138</f>
@@ -3237,10 +3238,10 @@
       <c r="A143" s="7"/>
       <c r="B143" s="14"/>
       <c r="C143" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D143" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="D143" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="E143" s="3">
         <f>D136-D141</f>
@@ -3257,7 +3258,7 @@
       <c r="B144" s="14"/>
       <c r="C144" s="3"/>
       <c r="D144" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E144" s="3">
         <f>D136+D141</f>
@@ -3276,7 +3277,7 @@
         <v>40</v>
       </c>
       <c r="D145" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E145" s="14"/>
       <c r="F145" s="14"/>

</xml_diff>